<commit_message>
changed tag button styling
</commit_message>
<xml_diff>
--- a/data/CategoriesAndTags.xlsx
+++ b/data/CategoriesAndTags.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tomar\source\repos\technical-blog\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{616C2520-FD12-4170-8384-0F020F91A450}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B982CFAC-8B79-4B4B-87B6-D6BFDAA3FD9C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28695" yWindow="0" windowWidth="29010" windowHeight="15585" xr2:uid="{71938F04-02B6-4E0B-A9C3-9D48821FDDCD}"/>
+    <workbookView xWindow="-105" yWindow="0" windowWidth="19410" windowHeight="15585" activeTab="1" xr2:uid="{71938F04-02B6-4E0B-A9C3-9D48821FDDCD}"/>
   </bookViews>
   <sheets>
     <sheet name="Categories" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="32">
   <si>
     <t>rain-paradox</t>
   </si>
@@ -108,9 +108,6 @@
     <t xml:space="preserve">OR-Tools </t>
   </si>
   <si>
-    <t xml:space="preserve">Meetings </t>
-  </si>
-  <si>
     <t>Opinion</t>
   </si>
   <si>
@@ -135,13 +132,7 @@
     <t>Guard Clause</t>
   </si>
   <si>
-    <t>Inverted-V</t>
-  </si>
-  <si>
     <t>Tag</t>
-  </si>
-  <si>
-    <t>Postt</t>
   </si>
 </sst>
 </file>
@@ -217,11 +208,10 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{98231BAD-8D29-4B43-9A96-9A801DC4069B}" name="Table2" displayName="Table2" ref="A1:B20" totalsRowShown="0">
-  <autoFilter ref="A1:B20" xr:uid="{98231BAD-8D29-4B43-9A96-9A801DC4069B}"/>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:B20">
-    <sortCondition ref="B2:B20"/>
-    <sortCondition ref="A2:A20"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{98231BAD-8D29-4B43-9A96-9A801DC4069B}" name="Table2" displayName="Table2" ref="A1:B16" totalsRowShown="0">
+  <autoFilter ref="A1:B16" xr:uid="{98231BAD-8D29-4B43-9A96-9A801DC4069B}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:B16">
+    <sortCondition ref="A1:A16"/>
   </sortState>
   <tableColumns count="2">
     <tableColumn id="1" xr3:uid="{F23996D8-E038-415A-AB46-54564A371285}" name="Category"/>
@@ -232,11 +222,14 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{07C3CC26-95B6-4B44-8B92-969D553E6E58}" name="Table3" displayName="Table3" ref="A1:B21" totalsRowShown="0">
-  <autoFilter ref="A1:B21" xr:uid="{07C3CC26-95B6-4B44-8B92-969D553E6E58}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{07C3CC26-95B6-4B44-8B92-969D553E6E58}" name="Table3" displayName="Table3" ref="A1:B24" totalsRowShown="0">
+  <autoFilter ref="A1:B24" xr:uid="{07C3CC26-95B6-4B44-8B92-969D553E6E58}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:B24">
+    <sortCondition ref="A1:A24"/>
+  </sortState>
   <tableColumns count="2">
     <tableColumn id="1" xr3:uid="{7A38640D-FB54-4A3A-B307-2BCDCDCF5A4D}" name="Tag"/>
-    <tableColumn id="2" xr3:uid="{9FA29049-8E81-4079-9D9A-737CCB3015ED}" name="Postt" dataDxfId="0"/>
+    <tableColumn id="2" xr3:uid="{9FA29049-8E81-4079-9D9A-737CCB3015ED}" name="Post" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -559,10 +552,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EEE28CF5-D7ED-41A9-98E3-4DEECEEA1CE1}">
-  <dimension ref="A1:B20"/>
+  <dimension ref="A1:B16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -588,15 +581,15 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B2" t="s">
-        <v>3</v>
+        <v>9</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="B3" t="s">
         <v>3</v>
@@ -604,18 +597,18 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>2</v>
+        <v>12</v>
       </c>
       <c r="B4" t="s">
-        <v>3</v>
+        <v>0</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>4</v>
+        <v>12</v>
       </c>
       <c r="B5" t="s">
-        <v>3</v>
+        <v>10</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
@@ -628,23 +621,23 @@
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="B7" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>4</v>
+        <v>17</v>
       </c>
       <c r="B8" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
       <c r="B9" t="s">
         <v>0</v>
@@ -655,86 +648,54 @@
         <v>17</v>
       </c>
       <c r="B10" t="s">
-        <v>0</v>
+        <v>10</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>2</v>
+        <v>17</v>
       </c>
       <c r="B11" t="s">
-        <v>0</v>
+        <v>9</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>4</v>
+        <v>23</v>
       </c>
       <c r="B12" t="s">
-        <v>0</v>
+        <v>9</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>13</v>
+        <v>2</v>
       </c>
       <c r="B13" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="B14" t="s">
-        <v>9</v>
+        <v>3</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>17</v>
+        <v>2</v>
       </c>
       <c r="B15" t="s">
-        <v>9</v>
+        <v>0</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>24</v>
+        <v>2</v>
       </c>
       <c r="B16" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
-        <v>12</v>
-      </c>
-      <c r="B17" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
-        <v>17</v>
-      </c>
-      <c r="B18" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
-        <v>2</v>
-      </c>
-      <c r="B19" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
-        <v>4</v>
-      </c>
-      <c r="B20" t="s">
         <v>10</v>
       </c>
     </row>
@@ -748,32 +709,32 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{27A5A7A2-6C88-4B5B-9CA2-1FC13B12127A}">
-  <dimension ref="A1:F21"/>
+  <dimension ref="A1:D24"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A18" sqref="A18:A21"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="18.28515625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="19.7109375" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="15.42578125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="18.42578125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="18.28515625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="12.42578125" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="19.7109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="15.42578125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="18.42578125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="18.28515625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="19.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>15</v>
       </c>
@@ -781,118 +742,117 @@
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
+        <v>28</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>20</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>30</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D5" s="1"/>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
         <v>16</v>
       </c>
-      <c r="B3" s="1" t="s">
+      <c r="B6" s="1" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>27</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>21</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
         <v>14</v>
       </c>
-      <c r="B4" s="1" t="s">
+      <c r="B9" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>14</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>14</v>
+      </c>
+      <c r="B11" s="1" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>27</v>
-      </c>
-      <c r="B5" s="1" t="s">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>26</v>
+      </c>
+      <c r="B12" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="D5" s="1"/>
-      <c r="F5" s="1"/>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>20</v>
-      </c>
-      <c r="B6" s="1" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>14</v>
-      </c>
-      <c r="B7" s="1" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>18</v>
-      </c>
-      <c r="B8" s="1" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>19</v>
-      </c>
-      <c r="B9" s="1" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>28</v>
-      </c>
-      <c r="B10" s="1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>21</v>
-      </c>
-      <c r="B11" s="1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
-        <v>14</v>
-      </c>
-      <c r="B12" s="1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B13" s="1" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>26</v>
+        <v>8</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>8</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>9</v>
+        <v>3</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
@@ -900,20 +860,20 @@
         <v>25</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>9</v>
+        <v>3</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>29</v>
+        <v>4</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>31</v>
+        <v>4</v>
       </c>
       <c r="B19" s="1" t="s">
         <v>6</v>
@@ -921,17 +881,41 @@
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>32</v>
+        <v>4</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>6</v>
+        <v>0</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>30</v>
+        <v>4</v>
       </c>
       <c r="B21" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>19</v>
+      </c>
+      <c r="B22" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>24</v>
+      </c>
+      <c r="B23" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>29</v>
+      </c>
+      <c r="B24" s="1" t="s">
         <v>6</v>
       </c>
     </row>

</xml_diff>